<commit_message>
mid-day update, the ScramjetEngine.m script works, however the code is very very slow, currently looking at ways we can speed this thing up.
</commit_message>
<xml_diff>
--- a/Cd_ss.xlsx
+++ b/Cd_ss.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cole\Documents\Grad School\PURDUE\AAE 53700\project\code\Repo\Hypersonics-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cole\Documents\Grad School\PURDUE\AAE 53700\project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Vehicle Geom" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0" concurrentManualCount="4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="96">
   <si>
     <t>Mach</t>
   </si>
@@ -307,15 +306,6 @@
   </si>
   <si>
     <t>M7</t>
-  </si>
-  <si>
-    <t>M4.5</t>
-  </si>
-  <si>
-    <t>M5.5</t>
-  </si>
-  <si>
-    <t>M6.5</t>
   </si>
   <si>
     <t>M4_5</t>
@@ -670,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,19 +677,19 @@
         <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
         <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>91</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I1" t="s">
         <v>92</v>

</xml_diff>